<commit_message>
Fixed GenerateRGBPalette; optimized Rainbow; tweaked InitStrip
</commit_message>
<xml_diff>
--- a/PhotonTorpedo.Device/Calculations.xlsx
+++ b/PhotonTorpedo.Device/Calculations.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lutz\VS Projects\Arduino\PhotonTorpedo\PhotonTorpedo\PhotonTorpedo.Device\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9660" activeTab="1"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,8 +70,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -95,9 +91,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -142,26 +138,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -969,7 +945,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-B02E-4992-8BB6-209DC77C938F}"/>
             </c:ext>
@@ -1775,7 +1751,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B02E-4992-8BB6-209DC77C938F}"/>
             </c:ext>
@@ -2581,7 +2557,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-B02E-4992-8BB6-209DC77C938F}"/>
             </c:ext>
@@ -2595,11 +2571,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2066153248"/>
-        <c:axId val="14824240"/>
+        <c:axId val="94760960"/>
+        <c:axId val="94762496"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2066153248"/>
+        <c:axId val="94760960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2641,7 +2617,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14824240"/>
+        <c:crossAx val="94762496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2649,7 +2625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14824240"/>
+        <c:axId val="94762496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2700,7 +2676,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2066153248"/>
+        <c:crossAx val="94760960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2745,14 +2721,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3363,7 +3339,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91579B79-405D-485C-98E4-87124039E2F2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91579B79-405D-485C-98E4-87124039E2F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3673,7 +3649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9094,13 +9070,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:U53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>16</v>
       </c>
@@ -9111,10 +9087,28 @@
         <v>16</v>
       </c>
       <c r="F1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="K1">
+        <v>4</v>
+      </c>
+      <c r="L1">
+        <v>16</v>
+      </c>
+      <c r="O1">
+        <v>20</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="S1">
+        <v>32</v>
+      </c>
+      <c r="T1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -9123,443 +9117,1583 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>MOD(B$1 * $A2, 16)</f>
+        <f t="shared" ref="C2:C17" si="0">MOD(B$1 * $A2, 16)</f>
         <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
-        <f>FLOOR(((F$1 + 1)/$A$1) * $A2, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f>MOD((F$1 + 1) * $A2, 16)</f>
+        <f>ROUNDDOWN(((F$1  * $E2)/$E$1), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <f>MOD((F$1 + G$1) * $E2, 16)</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>IF(G2&lt;=8,F2,IF(F2+1 &lt; $F$1, F2+1, 0)) + (G2 / $E$1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <f>F2 + (G2 / E$1)</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>G2*16</f>
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>ROUNDDOWN((K2 * L$1 / K$1), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>ROUNDDOWN(((K2 + 1) * L$1 / K$1), 0) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f>ROUNDDOWN((O2 * P$1 / O$1), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>ROUNDDOWN(((O2 + 1) * P$1 / O$1), 0) - 1</f>
+        <v>-1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <f>ROUNDDOWN((S2 * T$1 / S$1), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>ROUNDDOWN(((S2 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B17" si="0">ROUNDDOWN(((B$1 + 1)/$A$1) * $A3, 0)</f>
+        <f t="shared" ref="B3:B17" si="1">ROUNDDOWN(((B$1 + 1)/$A$1) * $A3, 0)</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f>MOD(B$1 * $A3, 16)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F17" si="1">ROUNDDOWN(((F$1 + 1)/$A$1) * $A3, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G17" si="2">MOD((F$1 + 1) * $A3, 16)</f>
+        <f t="shared" ref="F3:F17" si="2">ROUNDDOWN(((F$1  * $E3)/$E$1), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G17" si="3">MOD((F$1 + G$1) * $E3, 16)</f>
         <v>4</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H7" si="3">IF(G3&lt;=8,F3,IF(F3+1 &lt; $F$1, F3+1, 0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H3:H17" si="4">F3 + (G3 / E$1)</f>
+        <v>0.25</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="5">G3*16</f>
+        <v>64</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L5" si="6">ROUNDDOWN((K3 * L$1 / K$1), 0)</f>
+        <v>4</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M5" si="7">ROUNDDOWN(((K3 + 1) * L$1 / K$1), 0) - 1</f>
+        <v>7</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P21" si="8">ROUNDDOWN((O3 * P$1 / O$1), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q21" si="9">ROUNDDOWN(((O3 + 1) * P$1 / O$1), 0) - 1</f>
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T33" si="10">ROUNDDOWN((S3 * T$1 / S$1), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U33" si="11">ROUNDDOWN(((S3 + 1) * T$1 / S$1), 0) - 1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <f>MOD(B$1 * $A4, 16)</f>
         <v>6</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G4">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="H4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f>MOD(B$1 * $A5, 16)</f>
         <v>9</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G5">
         <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <f>MOD(B$1 * $A6, 16)</f>
         <v>12</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6">
-        <f>((F$1 + 1)/$A$1) * $A6</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
+      <c r="G6" s="1">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <f>MOD(B$1 * $A7, 16)</f>
         <v>15</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="4"/>
+        <v>1.25</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>16</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <f>MOD(B$1 * $A8, 16)</f>
         <v>2</v>
       </c>
       <c r="E8">
         <v>6</v>
       </c>
       <c r="F8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>ROUNDDOWN((K8 * L$7 / K$7), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>ROUNDDOWN(((K8 + 1) * L$7 / K$7), 0) - 1</f>
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>6</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>6</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="H8">
-        <f>IF(G8&lt;=8,F8,IF(F8+1 &lt; $F$1, F8+1, 0))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
+      <c r="C9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <f>MOD(B$1 * $A9, 16)</f>
         <v>5</v>
       </c>
       <c r="E9">
         <v>7</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
+      <c r="G9" s="1">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H9">
-        <f t="shared" ref="H9:H17" si="4">IF(G9&lt;=8,F9,IF(F9+1 &lt; $F$1, F9+1, 0))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>1.75</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L10" si="12">ROUNDDOWN((K9 * L$7 / K$7), 0)</f>
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ref="M9:M10" si="13">ROUNDDOWN(((K9 + 1) * L$7 / K$7), 0) - 1</f>
+        <v>9</v>
+      </c>
+      <c r="O9">
+        <v>7</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="10"/>
+        <v>3</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <f>MOD(B$1 * $A10, 16)</f>
         <v>8</v>
       </c>
       <c r="E10">
         <v>8</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
+      <c r="G10" s="1">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H10">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="O10">
+        <v>8</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="11"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <f>MOD(B$1 * $A11, 16)</f>
         <v>11</v>
       </c>
       <c r="E11">
         <v>9</v>
       </c>
       <c r="F11">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="4"/>
+        <v>2.25</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="O11">
+        <v>9</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="S11">
+        <v>9</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="10"/>
+        <v>4</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
+      <c r="C12">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <f>MOD(B$1 * $A12, 16)</f>
         <v>14</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="4"/>
+        <v>2.5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12">
+        <v>16</v>
+      </c>
+      <c r="O12">
+        <v>10</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="S12">
+        <v>10</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="11"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13">
+      <c r="C13">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <f>MOD(B$1 * $A13, 16)</f>
         <v>1</v>
       </c>
       <c r="E13">
         <v>11</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="2"/>
+      <c r="G13" s="1">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H13">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.75</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>ROUNDDOWN((K13 * L$12 / K$12), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>ROUNDDOWN(((K13 + 1) * L$12 / K$12), 0) - 1</f>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>11</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="9"/>
+        <v>8</v>
+      </c>
+      <c r="S13">
+        <v>11</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <f>MOD(B$1 * $A14, 16)</f>
         <v>4</v>
       </c>
       <c r="E14">
         <v>12</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="2"/>
+      <c r="G14" s="1">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H14">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L19" si="14">ROUNDDOWN((K14 * L$12 / K$12), 0)</f>
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14:M15" si="15">ROUNDDOWN(((K14 + 1) * L$12 / K$12), 0) - 1</f>
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>12</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="S14">
+        <v>12</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C15">
-        <f>MOD(B$1 * $A15, 16)</f>
         <v>7</v>
       </c>
       <c r="E15">
         <v>13</v>
       </c>
       <c r="F15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>3.25</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>64</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="14"/>
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>13</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="9"/>
+        <v>10</v>
+      </c>
+      <c r="S15">
+        <v>13</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="10"/>
+        <v>6</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16">
+      <c r="C16">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <f>MOD(B$1 * $A16, 16)</f>
         <v>10</v>
       </c>
       <c r="E16">
         <v>14</v>
       </c>
       <c r="F16">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>3.5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>128</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ref="M16:M19" si="16">ROUNDDOWN(((K16 + 1) * L$12 / K$12), 0) - 1</f>
+        <v>8</v>
+      </c>
+      <c r="O16">
+        <v>14</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="S16">
+        <v>14</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17">
+      <c r="C17">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <f>MOD(B$1 * $A17, 16)</f>
         <v>13</v>
       </c>
       <c r="E17">
         <v>15</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="2"/>
+      <c r="G17" s="1">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="H17">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3.75</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>192</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="16"/>
+        <v>10</v>
+      </c>
+      <c r="O17">
+        <v>15</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="S17">
+        <v>15</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="16"/>
+        <v>12</v>
+      </c>
+      <c r="O18">
+        <v>16</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="9"/>
+        <v>12</v>
+      </c>
+      <c r="S18">
+        <v>16</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>6</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+      <c r="O19">
+        <v>17</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="S19">
+        <v>17</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>255</v>
+      </c>
+      <c r="O20">
+        <v>18</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="S20">
+        <v>18</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="11"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <f>A20 * (1 - (A$21/A$20))</f>
+        <v>223</v>
+      </c>
+      <c r="O21">
+        <v>19</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="S21">
+        <v>19</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>A21-1</f>
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:B53" si="17">A21 * (1 - (A$21/A$20))</f>
+        <v>27.984313725490196</v>
+      </c>
+      <c r="S22">
+        <v>20</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" ref="A23:A36" si="18">A22-1</f>
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="17"/>
+        <v>27.109803921568627</v>
+      </c>
+      <c r="S23">
+        <v>21</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="10"/>
+        <v>10</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="18"/>
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="17"/>
+        <v>26.235294117647058</v>
+      </c>
+      <c r="S24">
+        <v>22</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="11"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="18"/>
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="17"/>
+        <v>25.360784313725489</v>
+      </c>
+      <c r="S25">
+        <v>23</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="11"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="18"/>
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="17"/>
+        <v>24.48627450980392</v>
+      </c>
+      <c r="S26">
+        <v>24</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="11"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="18"/>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="17"/>
+        <v>23.611764705882354</v>
+      </c>
+      <c r="S27">
+        <v>25</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="10"/>
+        <v>12</v>
+      </c>
+      <c r="U27">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="18"/>
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="17"/>
+        <v>22.737254901960785</v>
+      </c>
+      <c r="S28">
+        <v>26</v>
+      </c>
+      <c r="T28">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="U28">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="18"/>
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="17"/>
+        <v>21.862745098039216</v>
+      </c>
+      <c r="S29">
+        <v>27</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="18"/>
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="17"/>
+        <v>20.988235294117647</v>
+      </c>
+      <c r="S30">
+        <v>28</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="18"/>
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="17"/>
+        <v>20.113725490196078</v>
+      </c>
+      <c r="S31">
+        <v>29</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="10"/>
+        <v>14</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="18"/>
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="17"/>
+        <v>19.239215686274509</v>
+      </c>
+      <c r="S32">
+        <v>30</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="18"/>
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="17"/>
+        <v>18.36470588235294</v>
+      </c>
+      <c r="S33">
+        <v>31</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="18"/>
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="17"/>
+        <v>17.490196078431374</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="18"/>
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="17"/>
+        <v>16.615686274509805</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="18"/>
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="17"/>
+        <v>15.741176470588236</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" ref="A37" si="19">A36-1</f>
+        <v>16</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="17"/>
+        <v>14.866666666666667</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" ref="A38:A51" si="20">A37-1</f>
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="17"/>
+        <v>13.992156862745098</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="20"/>
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="17"/>
+        <v>13.117647058823529</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="20"/>
+        <v>13</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="17"/>
+        <v>12.24313725490196</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="20"/>
+        <v>12</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="17"/>
+        <v>11.368627450980393</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="20"/>
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="17"/>
+        <v>10.494117647058824</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="17"/>
+        <v>9.6196078431372545</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="20"/>
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="17"/>
+        <v>8.7450980392156872</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="17"/>
+        <v>7.8705882352941181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="17"/>
+        <v>6.996078431372549</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="20"/>
+        <v>6</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="17"/>
+        <v>6.12156862745098</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="17"/>
+        <v>5.2470588235294118</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="20"/>
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="17"/>
+        <v>4.3725490196078436</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="17"/>
+        <v>3.4980392156862745</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="17"/>
+        <v>2.6235294117647059</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" ref="A52:A53" si="21">A51-1</f>
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="17"/>
+        <v>1.7490196078431373</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="17"/>
+        <v>0.87450980392156863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>